<commit_message>
modify StudyLevel G11 Literaty
</commit_message>
<xml_diff>
--- a/Yemen -General Education-literary -level 11.xlsx
+++ b/Yemen -General Education-literary -level 11.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private3\My Work\AppNest\Mozakarah\Subjects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdel\Downloads\Mozakara Python Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52ABFA0A-06A0-4C06-9CCF-BD798F030B58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4944B8D7-85A9-4763-BA6F-01EF654A0CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{5C29EAFA-30EB-4F60-83F5-14B1783D3A75}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5C29EAFA-30EB-4F60-83F5-14B1783D3A75}"/>
   </bookViews>
   <sheets>
     <sheet name="Lessons" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="744">
   <si>
     <t>Id</t>
   </si>
@@ -2265,6 +2270,9 @@
   </si>
   <si>
     <t xml:space="preserve">يتناول الدرس : نسب علي بن أبي طالب , ونشأته , ويذكر أمثلة على شجاعته وبطولاته , وزهده وعلمه وورعه , ويبين دوره في خدمة الإسلام ,  ويوضح أسباب استشهاده . </t>
+  </si>
+  <si>
+    <t>9f054d20-191e-4b85-892b-d41d1f861e6d</t>
   </si>
 </sst>
 </file>
@@ -2725,7 +2733,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="اسلامية ثاني أدبي"/>
@@ -5322,9 +5330,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5362,7 +5370,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5468,7 +5476,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5610,7 +5618,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5626,26 +5634,26 @@
       <selection pane="bottomLeft" activeCell="M301" sqref="M301:N309"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.1796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.26953125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="54.26953125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="21.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.08984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.7265625" style="11"/>
+    <col min="1" max="1" width="43.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.21875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="54.21875" style="12" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.77734375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -5689,7 +5697,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="37"/>
       <c r="B2" s="1">
         <v>60</v>
@@ -5733,7 +5741,7 @@
         <v>الإنسان اليمني وبيئته الطبيعية</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>60</v>
       </c>
@@ -5776,7 +5784,7 @@
         <v>الإنسان اليمني وبيئته الطبيعية</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>60</v>
       </c>
@@ -5819,7 +5827,7 @@
         <v>الإنسان اليمني وبيئته الطبيعية</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>60</v>
       </c>
@@ -5862,7 +5870,7 @@
         <v>الإنسان اليمني وبيئته الطبيعية</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>60</v>
       </c>
@@ -5905,7 +5913,7 @@
         <v>الإنسان اليمني وبيئته الطبيعية</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>60</v>
       </c>
@@ -5948,7 +5956,7 @@
         <v>الإنسان اليمني وبيئته الطبيعية</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>60</v>
       </c>
@@ -5991,7 +5999,7 @@
         <v>السكان والتنمية الاجتماعية في اليمن</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>60</v>
       </c>
@@ -6034,7 +6042,7 @@
         <v>السكان والتنمية الاجتماعية في اليمن</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="92.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="90" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>60</v>
       </c>
@@ -6077,7 +6085,7 @@
         <v>السكان والتنمية الاجتماعية في اليمن</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>60</v>
       </c>
@@ -6120,7 +6128,7 @@
         <v>السكان والتنمية الاجتماعية في اليمن</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>60</v>
       </c>
@@ -6163,7 +6171,7 @@
         <v>السكان والتنمية الاجتماعية في اليمن</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>60</v>
       </c>
@@ -6206,7 +6214,7 @@
         <v>السكان والتنمية الاجتماعية في اليمن</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>60</v>
       </c>
@@ -6249,7 +6257,7 @@
         <v>السكان والتنمية الاجتماعية في اليمن</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>60</v>
       </c>
@@ -6292,7 +6300,7 @@
         <v>موارد اليمن الاقتصادية</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>60</v>
       </c>
@@ -6335,7 +6343,7 @@
         <v>موارد اليمن الاقتصادية</v>
       </c>
     </row>
-    <row r="17" spans="2:14" ht="92.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:14" ht="90" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>60</v>
       </c>
@@ -6378,7 +6386,7 @@
         <v>موارد اليمن الاقتصادية</v>
       </c>
     </row>
-    <row r="18" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>60</v>
       </c>
@@ -6421,7 +6429,7 @@
         <v>موارد اليمن الاقتصادية</v>
       </c>
     </row>
-    <row r="19" spans="2:14" ht="92.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:14" ht="90" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>60</v>
       </c>
@@ -6464,7 +6472,7 @@
         <v>موارد اليمن الاقتصادية</v>
       </c>
     </row>
-    <row r="20" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>60</v>
       </c>
@@ -6507,7 +6515,7 @@
         <v>موارد اليمن الاقتصادية</v>
       </c>
     </row>
-    <row r="21" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
         <v>60</v>
       </c>
@@ -6550,7 +6558,7 @@
         <v>الجغرافية الطبيعية للوطن العربي</v>
       </c>
     </row>
-    <row r="22" spans="2:14" ht="92.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:14" ht="90" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
         <v>60</v>
       </c>
@@ -6593,7 +6601,7 @@
         <v>الجغرافية الطبيعية للوطن العربي</v>
       </c>
     </row>
-    <row r="23" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>60</v>
       </c>
@@ -6636,7 +6644,7 @@
         <v>الجغرافية الطبيعية للوطن العربي</v>
       </c>
     </row>
-    <row r="24" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
         <v>60</v>
       </c>
@@ -6679,7 +6687,7 @@
         <v>الجغرافية الطبيعية للوطن العربي</v>
       </c>
     </row>
-    <row r="25" spans="2:14" ht="92.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:14" ht="90" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
         <v>60</v>
       </c>
@@ -6722,7 +6730,7 @@
         <v>سكان الوطن العربي ومواردهم الاقتصادية</v>
       </c>
     </row>
-    <row r="26" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>60</v>
       </c>
@@ -6765,7 +6773,7 @@
         <v>سكان الوطن العربي ومواردهم الاقتصادية</v>
       </c>
     </row>
-    <row r="27" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
         <v>60</v>
       </c>
@@ -6808,7 +6816,7 @@
         <v>سكان الوطن العربي ومواردهم الاقتصادية</v>
       </c>
     </row>
-    <row r="28" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
         <v>60</v>
       </c>
@@ -6851,7 +6859,7 @@
         <v>سكان الوطن العربي ومواردهم الاقتصادية</v>
       </c>
     </row>
-    <row r="29" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
         <v>60</v>
       </c>
@@ -6894,7 +6902,7 @@
         <v>سكان الوطن العربي ومواردهم الاقتصادية</v>
       </c>
     </row>
-    <row r="30" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B30" s="1">
         <v>60</v>
       </c>
@@ -6937,7 +6945,7 @@
         <v>سكان الوطن العربي ومواردهم الاقتصادية</v>
       </c>
     </row>
-    <row r="31" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B31" s="1">
         <v>60</v>
       </c>
@@ -6980,7 +6988,7 @@
         <v>سكان الوطن العربي ومواردهم الاقتصادية</v>
       </c>
     </row>
-    <row r="32" spans="2:14" ht="92.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:14" ht="90" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
         <v>60</v>
       </c>
@@ -7023,7 +7031,7 @@
         <v>مشكلات وقضايا معاصرة في الوطن العربي</v>
       </c>
     </row>
-    <row r="33" spans="2:14" ht="92.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:14" ht="90" x14ac:dyDescent="0.3">
       <c r="B33" s="1">
         <v>60</v>
       </c>
@@ -7066,7 +7074,7 @@
         <v>مشكلات وقضايا معاصرة في الوطن العربي</v>
       </c>
     </row>
-    <row r="34" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B34" s="1">
         <v>60</v>
       </c>
@@ -7109,7 +7117,7 @@
         <v>مشكلات وقضايا معاصرة في الوطن العربي</v>
       </c>
     </row>
-    <row r="35" spans="2:14" ht="111" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:14" ht="108" x14ac:dyDescent="0.3">
       <c r="B35" s="1">
         <v>60</v>
       </c>
@@ -7152,7 +7160,7 @@
         <v>مشكلات وقضايا معاصرة في الوطن العربي</v>
       </c>
     </row>
-    <row r="36" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B36" s="1">
         <v>60</v>
       </c>
@@ -7195,7 +7203,7 @@
         <v>مشكلات وقضايا معاصرة في الوطن العربي</v>
       </c>
     </row>
-    <row r="37" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B37" s="1">
         <v>60</v>
       </c>
@@ -7238,7 +7246,7 @@
         <v>مشكلات وقضايا معاصرة في الوطن العربي</v>
       </c>
     </row>
-    <row r="38" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B38" s="1">
         <v>60</v>
       </c>
@@ -7281,7 +7289,7 @@
         <v>مشكلات وقضايا معاصرة في الوطن العربي</v>
       </c>
     </row>
-    <row r="39" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B39" s="1">
         <v>60</v>
       </c>
@@ -7324,7 +7332,7 @@
         <v>الحضارة العربية الإسلامية</v>
       </c>
     </row>
-    <row r="40" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B40" s="1">
         <v>60</v>
       </c>
@@ -7367,7 +7375,7 @@
         <v>الحضارة العربية الإسلامية</v>
       </c>
     </row>
-    <row r="41" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B41" s="1">
         <v>60</v>
       </c>
@@ -7410,7 +7418,7 @@
         <v>الحضارة العربية الإسلامية</v>
       </c>
     </row>
-    <row r="42" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B42" s="1">
         <v>60</v>
       </c>
@@ -7453,7 +7461,7 @@
         <v>الحضارة العربية الإسلامية</v>
       </c>
     </row>
-    <row r="43" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B43" s="1">
         <v>60</v>
       </c>
@@ -7496,7 +7504,7 @@
         <v>التطور التاريخي للحضارة العربية الإسلامية</v>
       </c>
     </row>
-    <row r="44" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B44" s="1">
         <v>60</v>
       </c>
@@ -7539,7 +7547,7 @@
         <v>التطور التاريخي للحضارة العربية الإسلامية</v>
       </c>
     </row>
-    <row r="45" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B45" s="1">
         <v>60</v>
       </c>
@@ -7582,7 +7590,7 @@
         <v>التطور التاريخي للحضارة العربية الإسلامية</v>
       </c>
     </row>
-    <row r="46" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B46" s="1">
         <v>60</v>
       </c>
@@ -7625,7 +7633,7 @@
         <v>التطور التاريخي للحضارة العربية الإسلامية</v>
       </c>
     </row>
-    <row r="47" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B47" s="1">
         <v>60</v>
       </c>
@@ -7668,7 +7676,7 @@
         <v>التطور التاريخي للحضارة العربية الإسلامية</v>
       </c>
     </row>
-    <row r="48" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B48" s="1">
         <v>60</v>
       </c>
@@ -7711,7 +7719,7 @@
         <v>التطور التاريخي للحضارة العربية الإسلامية</v>
       </c>
     </row>
-    <row r="49" spans="2:14" ht="92.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:14" ht="90" x14ac:dyDescent="0.3">
       <c r="B49" s="1">
         <v>60</v>
       </c>
@@ -7754,7 +7762,7 @@
         <v>جذور الشورى والديمقراطية في الحضارة العربية والإسلامية</v>
       </c>
     </row>
-    <row r="50" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B50" s="1">
         <v>60</v>
       </c>
@@ -7797,7 +7805,7 @@
         <v>جذور الشورى والديمقراطية في الحضارة العربية والإسلامية</v>
       </c>
     </row>
-    <row r="51" spans="2:14" ht="92.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:14" ht="90" x14ac:dyDescent="0.3">
       <c r="B51" s="1">
         <v>60</v>
       </c>
@@ -7840,7 +7848,7 @@
         <v>جذور الشورى والديمقراطية في الحضارة العربية والإسلامية</v>
       </c>
     </row>
-    <row r="52" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B52" s="1">
         <v>60</v>
       </c>
@@ -7883,7 +7891,7 @@
         <v>جذور الشورى والديمقراطية في الحضارة العربية والإسلامية</v>
       </c>
     </row>
-    <row r="53" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B53" s="1">
         <v>60</v>
       </c>
@@ -7926,7 +7934,7 @@
         <v>جذور الشورى والديمقراطية في الحضارة العربية والإسلامية</v>
       </c>
     </row>
-    <row r="54" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B54" s="1">
         <v>60</v>
       </c>
@@ -7969,7 +7977,7 @@
         <v>جذور الشورى والديمقراطية في الحضارة العربية والإسلامية</v>
       </c>
     </row>
-    <row r="55" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B55" s="1">
         <v>60</v>
       </c>
@@ -8012,7 +8020,7 @@
         <v>علم الاجتماع والعلوم الاجتماعية الأخرى</v>
       </c>
     </row>
-    <row r="56" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B56" s="1">
         <v>60</v>
       </c>
@@ -8055,7 +8063,7 @@
         <v>علم الاجتماع والعلوم الاجتماعية الأخرى</v>
       </c>
     </row>
-    <row r="57" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B57" s="1">
         <v>60</v>
       </c>
@@ -8098,7 +8106,7 @@
         <v>علم الاجتماع والعلوم الاجتماعية الأخرى</v>
       </c>
     </row>
-    <row r="58" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B58" s="1">
         <v>60</v>
       </c>
@@ -8141,7 +8149,7 @@
         <v>علم الاجتماع والعلوم الاجتماعية الأخرى</v>
       </c>
     </row>
-    <row r="59" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B59" s="1">
         <v>60</v>
       </c>
@@ -8184,7 +8192,7 @@
         <v>رواد علم الاجتماع</v>
       </c>
     </row>
-    <row r="60" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B60" s="1">
         <v>60</v>
       </c>
@@ -8227,7 +8235,7 @@
         <v>رواد علم الاجتماع</v>
       </c>
     </row>
-    <row r="61" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B61" s="1">
         <v>60</v>
       </c>
@@ -8270,7 +8278,7 @@
         <v>رواد علم الاجتماع</v>
       </c>
     </row>
-    <row r="62" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B62" s="1">
         <v>60</v>
       </c>
@@ -8313,7 +8321,7 @@
         <v>رواد علم الاجتماع</v>
       </c>
     </row>
-    <row r="63" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B63" s="1">
         <v>60</v>
       </c>
@@ -8356,7 +8364,7 @@
         <v>مناهج البحث الاجتماعي</v>
       </c>
     </row>
-    <row r="64" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B64" s="1">
         <v>60</v>
       </c>
@@ -8399,7 +8407,7 @@
         <v>مناهج البحث الاجتماعي</v>
       </c>
     </row>
-    <row r="65" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B65" s="1">
         <v>60</v>
       </c>
@@ -8442,7 +8450,7 @@
         <v>مناهج البحث الاجتماعي</v>
       </c>
     </row>
-    <row r="66" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B66" s="1">
         <v>60</v>
       </c>
@@ -8485,7 +8493,7 @@
         <v>مناهج البحث الاجتماعي</v>
       </c>
     </row>
-    <row r="67" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B67" s="1">
         <v>60</v>
       </c>
@@ -8528,7 +8536,7 @@
         <v>مناهج البحث الاجتماعي</v>
       </c>
     </row>
-    <row r="68" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B68" s="1">
         <v>60</v>
       </c>
@@ -8571,7 +8579,7 @@
         <v>النطم والعلاقات الاجتماعية</v>
       </c>
     </row>
-    <row r="69" spans="2:14" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B69" s="1">
         <v>60</v>
       </c>
@@ -8614,7 +8622,7 @@
         <v>النطم والعلاقات الاجتماعية</v>
       </c>
     </row>
-    <row r="70" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B70" s="1">
         <v>60</v>
       </c>
@@ -8657,7 +8665,7 @@
         <v>النطم والعلاقات الاجتماعية</v>
       </c>
     </row>
-    <row r="71" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B71" s="1">
         <v>60</v>
       </c>
@@ -8700,7 +8708,7 @@
         <v>التنشئة الاجتماعية والظبط الاجتماعي</v>
       </c>
     </row>
-    <row r="72" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B72" s="1">
         <v>60</v>
       </c>
@@ -8743,7 +8751,7 @@
         <v>التنشئة الاجتماعية والظبط الاجتماعي</v>
       </c>
     </row>
-    <row r="73" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B73" s="1">
         <v>60</v>
       </c>
@@ -8786,7 +8794,7 @@
         <v>التنشئة الاجتماعية والظبط الاجتماعي</v>
       </c>
     </row>
-    <row r="74" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B74" s="1">
         <v>60</v>
       </c>
@@ -8829,7 +8837,7 @@
         <v>التغيير الاجتماعي</v>
       </c>
     </row>
-    <row r="75" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B75" s="1">
         <v>60</v>
       </c>
@@ -8872,7 +8880,7 @@
         <v>التغيير الاجتماعي</v>
       </c>
     </row>
-    <row r="76" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B76" s="1">
         <v>60</v>
       </c>
@@ -8915,7 +8923,7 @@
         <v>التغيير الاجتماعي</v>
       </c>
     </row>
-    <row r="77" spans="2:14" ht="111" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:14" ht="108" x14ac:dyDescent="0.3">
       <c r="B77" s="1">
         <v>60</v>
       </c>
@@ -8958,7 +8966,7 @@
         <v>الفكر الاقتصادي وعلم الاقتصاد</v>
       </c>
     </row>
-    <row r="78" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B78" s="1">
         <v>60</v>
       </c>
@@ -9001,7 +9009,7 @@
         <v>الفكر الاقتصادي وعلم الاقتصاد</v>
       </c>
     </row>
-    <row r="79" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B79" s="1">
         <v>60</v>
       </c>
@@ -9044,7 +9052,7 @@
         <v>الفكر الاقتصادي وعلم الاقتصاد</v>
       </c>
     </row>
-    <row r="80" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B80" s="1">
         <v>60</v>
       </c>
@@ -9087,7 +9095,7 @@
         <v>الفكر الاقتصادي وعلم الاقتصاد</v>
       </c>
     </row>
-    <row r="81" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B81" s="1">
         <v>60</v>
       </c>
@@ -9130,7 +9138,7 @@
         <v>المشكلة الاقتصادية وعناصرها</v>
       </c>
     </row>
-    <row r="82" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B82" s="1">
         <v>60</v>
       </c>
@@ -9173,7 +9181,7 @@
         <v>المشكلة الاقتصادية وعناصرها</v>
       </c>
     </row>
-    <row r="83" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B83" s="1">
         <v>60</v>
       </c>
@@ -9216,7 +9224,7 @@
         <v>المشكلة الاقتصادية وعناصرها</v>
       </c>
     </row>
-    <row r="84" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B84" s="1">
         <v>60</v>
       </c>
@@ -9259,7 +9267,7 @@
         <v>المشكلة الاقتصادية وعناصرها</v>
       </c>
     </row>
-    <row r="85" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B85" s="1">
         <v>60</v>
       </c>
@@ -9302,7 +9310,7 @@
         <v>عناصر الإنتاج</v>
       </c>
     </row>
-    <row r="86" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B86" s="1">
         <v>60</v>
       </c>
@@ -9345,7 +9353,7 @@
         <v>عناصر الإنتاج</v>
       </c>
     </row>
-    <row r="87" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B87" s="1">
         <v>60</v>
       </c>
@@ -9388,7 +9396,7 @@
         <v>عناصر الإنتاج</v>
       </c>
     </row>
-    <row r="88" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B88" s="1">
         <v>60</v>
       </c>
@@ -9431,7 +9439,7 @@
         <v>عناصر الإنتاج</v>
       </c>
     </row>
-    <row r="89" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B89" s="1">
         <v>60</v>
       </c>
@@ -9474,7 +9482,7 @@
         <v>عناصر الإنتاج</v>
       </c>
     </row>
-    <row r="90" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B90" s="1">
         <v>60</v>
       </c>
@@ -9517,7 +9525,7 @@
         <v>طلب وعرض السوق</v>
       </c>
     </row>
-    <row r="91" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B91" s="1">
         <v>60</v>
       </c>
@@ -9560,7 +9568,7 @@
         <v>طلب وعرض السوق</v>
       </c>
     </row>
-    <row r="92" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B92" s="1">
         <v>60</v>
       </c>
@@ -9603,7 +9611,7 @@
         <v>طلب وعرض السوق</v>
       </c>
     </row>
-    <row r="93" spans="2:14" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:14" ht="18" x14ac:dyDescent="0.3">
       <c r="B93" s="1">
         <v>60</v>
       </c>
@@ -9646,7 +9654,7 @@
         <v>طلب وعرض السوق</v>
       </c>
     </row>
-    <row r="94" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B94" s="1">
         <v>60</v>
       </c>
@@ -9689,7 +9697,7 @@
         <v>طلب وعرض السوق</v>
       </c>
     </row>
-    <row r="95" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B95" s="1">
         <v>60</v>
       </c>
@@ -9732,7 +9740,7 @@
         <v>النقود والبنوك</v>
       </c>
     </row>
-    <row r="96" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B96" s="1">
         <v>60</v>
       </c>
@@ -9775,7 +9783,7 @@
         <v>النقود والبنوك</v>
       </c>
     </row>
-    <row r="97" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B97" s="1">
         <v>60</v>
       </c>
@@ -9818,7 +9826,7 @@
         <v>النقود والبنوك</v>
       </c>
     </row>
-    <row r="98" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B98" s="1">
         <v>60</v>
       </c>
@@ -9861,7 +9869,7 @@
         <v>الحفظ والتفسير 1</v>
       </c>
     </row>
-    <row r="99" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B99" s="1">
         <v>60</v>
       </c>
@@ -9904,7 +9912,7 @@
         <v>الحفظ والتفسير 1</v>
       </c>
     </row>
-    <row r="100" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B100" s="1">
         <v>60</v>
       </c>
@@ -9947,7 +9955,7 @@
         <v>الحفظ والتفسير 1</v>
       </c>
     </row>
-    <row r="101" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B101" s="1">
         <v>60</v>
       </c>
@@ -9990,7 +9998,7 @@
         <v>الحفظ والتفسير 1</v>
       </c>
     </row>
-    <row r="102" spans="2:14" ht="92.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:14" ht="90" x14ac:dyDescent="0.3">
       <c r="B102" s="1">
         <v>60</v>
       </c>
@@ -10033,7 +10041,7 @@
         <v>الحفظ والتفسير 1</v>
       </c>
     </row>
-    <row r="103" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B103" s="1">
         <v>60</v>
       </c>
@@ -10076,7 +10084,7 @@
         <v>الحفظ والتفسير 1</v>
       </c>
     </row>
-    <row r="104" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B104" s="1">
         <v>60</v>
       </c>
@@ -10119,7 +10127,7 @@
         <v>الحفظ والتفسير 1</v>
       </c>
     </row>
-    <row r="105" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B105" s="1">
         <v>60</v>
       </c>
@@ -10162,7 +10170,7 @@
         <v>علوم القرآن 1</v>
       </c>
     </row>
-    <row r="106" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B106" s="1">
         <v>60</v>
       </c>
@@ -10205,7 +10213,7 @@
         <v>علوم القرآن 1</v>
       </c>
     </row>
-    <row r="107" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B107" s="1">
         <v>60</v>
       </c>
@@ -10248,7 +10256,7 @@
         <v>علوم القرآن 1</v>
       </c>
     </row>
-    <row r="108" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B108" s="1">
         <v>60</v>
       </c>
@@ -10291,7 +10299,7 @@
         <v>التلاوة 1</v>
       </c>
     </row>
-    <row r="109" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B109" s="1">
         <v>60</v>
       </c>
@@ -10334,7 +10342,7 @@
         <v>التلاوة 1</v>
       </c>
     </row>
-    <row r="110" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B110" s="1">
         <v>60</v>
       </c>
@@ -10377,7 +10385,7 @@
         <v>التلاوة 1</v>
       </c>
     </row>
-    <row r="111" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B111" s="1">
         <v>60</v>
       </c>
@@ -10420,7 +10428,7 @@
         <v>التلاوة 1</v>
       </c>
     </row>
-    <row r="112" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B112" s="1">
         <v>60</v>
       </c>
@@ -10463,7 +10471,7 @@
         <v>التلاوة 1</v>
       </c>
     </row>
-    <row r="113" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B113" s="1">
         <v>60</v>
       </c>
@@ -10506,7 +10514,7 @@
         <v>التلاوة 1</v>
       </c>
     </row>
-    <row r="114" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B114" s="1">
         <v>60</v>
       </c>
@@ -10549,7 +10557,7 @@
         <v>التلاوة 1</v>
       </c>
     </row>
-    <row r="115" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B115" s="1">
         <v>60</v>
       </c>
@@ -10592,7 +10600,7 @@
         <v>التلاوة 1</v>
       </c>
     </row>
-    <row r="116" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B116" s="1">
         <v>60</v>
       </c>
@@ -10635,7 +10643,7 @@
         <v>التلاوة 1</v>
       </c>
     </row>
-    <row r="117" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B117" s="1">
         <v>60</v>
       </c>
@@ -10678,7 +10686,7 @@
         <v>التلاوة 1</v>
       </c>
     </row>
-    <row r="118" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B118" s="1">
         <v>60</v>
       </c>
@@ -10721,7 +10729,7 @@
         <v>الحفظ والتفسير 2</v>
       </c>
     </row>
-    <row r="119" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B119" s="1">
         <v>60</v>
       </c>
@@ -10764,7 +10772,7 @@
         <v>الحفظ والتفسير 2</v>
       </c>
     </row>
-    <row r="120" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="120" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B120" s="1">
         <v>60</v>
       </c>
@@ -10807,7 +10815,7 @@
         <v>الحفظ والتفسير 2</v>
       </c>
     </row>
-    <row r="121" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B121" s="1">
         <v>60</v>
       </c>
@@ -10850,7 +10858,7 @@
         <v>الحفظ والتفسير 2</v>
       </c>
     </row>
-    <row r="122" spans="2:14" ht="92.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:14" ht="90" x14ac:dyDescent="0.3">
       <c r="B122" s="1">
         <v>60</v>
       </c>
@@ -10893,7 +10901,7 @@
         <v>الحفظ والتفسير 2</v>
       </c>
     </row>
-    <row r="123" spans="2:14" ht="92.5" x14ac:dyDescent="0.45">
+    <row r="123" spans="2:14" ht="90" x14ac:dyDescent="0.35">
       <c r="B123" s="1">
         <v>60</v>
       </c>
@@ -10936,7 +10944,7 @@
         <v>الحفظ والتفسير 2</v>
       </c>
     </row>
-    <row r="124" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B124" s="1">
         <v>60</v>
       </c>
@@ -10979,7 +10987,7 @@
         <v>الحفظ والتفسير 2</v>
       </c>
     </row>
-    <row r="125" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="125" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B125" s="1">
         <v>60</v>
       </c>
@@ -11022,7 +11030,7 @@
         <v>علوم القرآن 2</v>
       </c>
     </row>
-    <row r="126" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="126" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B126" s="1">
         <v>60</v>
       </c>
@@ -11065,7 +11073,7 @@
         <v>علوم القرآن 2</v>
       </c>
     </row>
-    <row r="127" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="127" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B127" s="1">
         <v>60</v>
       </c>
@@ -11108,7 +11116,7 @@
         <v>علوم القرآن 2</v>
       </c>
     </row>
-    <row r="128" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="128" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B128" s="1">
         <v>60</v>
       </c>
@@ -11151,7 +11159,7 @@
         <v>التلاوة 2</v>
       </c>
     </row>
-    <row r="129" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="129" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B129" s="1">
         <v>60</v>
       </c>
@@ -11194,7 +11202,7 @@
         <v>التلاوة 2</v>
       </c>
     </row>
-    <row r="130" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="130" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B130" s="1">
         <v>60</v>
       </c>
@@ -11237,7 +11245,7 @@
         <v>التلاوة 2</v>
       </c>
     </row>
-    <row r="131" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="131" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B131" s="1">
         <v>60</v>
       </c>
@@ -11280,7 +11288,7 @@
         <v>التلاوة 2</v>
       </c>
     </row>
-    <row r="132" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="132" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B132" s="1">
         <v>60</v>
       </c>
@@ -11323,7 +11331,7 @@
         <v>التلاوة 2</v>
       </c>
     </row>
-    <row r="133" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="133" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B133" s="1">
         <v>60</v>
       </c>
@@ -11366,7 +11374,7 @@
         <v>التلاوة 2</v>
       </c>
     </row>
-    <row r="134" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="134" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B134" s="1">
         <v>60</v>
       </c>
@@ -11409,7 +11417,7 @@
         <v>التلاوة 2</v>
       </c>
     </row>
-    <row r="135" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="135" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B135" s="1">
         <v>60</v>
       </c>
@@ -11452,7 +11460,7 @@
         <v>التلاوة 2</v>
       </c>
     </row>
-    <row r="136" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="136" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B136" s="1">
         <v>60</v>
       </c>
@@ -11495,7 +11503,7 @@
         <v>التلاوة 2</v>
       </c>
     </row>
-    <row r="137" spans="2:14" ht="37.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="137" spans="2:14" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B137" s="1">
         <v>60</v>
       </c>
@@ -11538,7 +11546,7 @@
         <v>التلاوة 2</v>
       </c>
     </row>
-    <row r="138" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="138" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B138" s="1">
         <v>60</v>
       </c>
@@ -11581,7 +11589,7 @@
         <v>المتتاليات</v>
       </c>
     </row>
-    <row r="139" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="139" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B139" s="1">
         <v>60</v>
       </c>
@@ -11624,7 +11632,7 @@
         <v>المتتاليات</v>
       </c>
     </row>
-    <row r="140" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="140" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B140" s="1">
         <v>60</v>
       </c>
@@ -11667,7 +11675,7 @@
         <v>المتتاليات</v>
       </c>
     </row>
-    <row r="141" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="141" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B141" s="1">
         <v>60</v>
       </c>
@@ -11710,7 +11718,7 @@
         <v>المتتاليات</v>
       </c>
     </row>
-    <row r="142" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="142" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B142" s="1">
         <v>60</v>
       </c>
@@ -11753,7 +11761,7 @@
         <v>المتتاليات</v>
       </c>
     </row>
-    <row r="143" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="143" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B143" s="1">
         <v>60</v>
       </c>
@@ -11796,7 +11804,7 @@
         <v>اللوغاريتمات</v>
       </c>
     </row>
-    <row r="144" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="144" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B144" s="1">
         <v>60</v>
       </c>
@@ -11839,7 +11847,7 @@
         <v>اللوغاريتمات</v>
       </c>
     </row>
-    <row r="145" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="145" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B145" s="1">
         <v>60</v>
       </c>
@@ -11882,7 +11890,7 @@
         <v>اللوغاريتمات</v>
       </c>
     </row>
-    <row r="146" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="146" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B146" s="1">
         <v>60</v>
       </c>
@@ -11925,7 +11933,7 @@
         <v>اللوغاريتمات</v>
       </c>
     </row>
-    <row r="147" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="147" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B147" s="1">
         <v>60</v>
       </c>
@@ -11968,7 +11976,7 @@
         <v>اللوغاريتمات</v>
       </c>
     </row>
-    <row r="148" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="148" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B148" s="1">
         <v>60</v>
       </c>
@@ -12011,7 +12019,7 @@
         <v>المصفوفات والمحددات</v>
       </c>
     </row>
-    <row r="149" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="149" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B149" s="1">
         <v>60</v>
       </c>
@@ -12054,7 +12062,7 @@
         <v>المصفوفات والمحددات</v>
       </c>
     </row>
-    <row r="150" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="150" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B150" s="1">
         <v>60</v>
       </c>
@@ -12097,7 +12105,7 @@
         <v>المصفوفات والمحددات</v>
       </c>
     </row>
-    <row r="151" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="151" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B151" s="1">
         <v>60</v>
       </c>
@@ -12140,7 +12148,7 @@
         <v>المصفوفات والمحددات</v>
       </c>
     </row>
-    <row r="152" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="152" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B152" s="1">
         <v>60</v>
       </c>
@@ -12183,7 +12191,7 @@
         <v>المشتقات</v>
       </c>
     </row>
-    <row r="153" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="153" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B153" s="1">
         <v>60</v>
       </c>
@@ -12226,7 +12234,7 @@
         <v>المشتقات</v>
       </c>
     </row>
-    <row r="154" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="154" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B154" s="1">
         <v>60</v>
       </c>
@@ -12269,7 +12277,7 @@
         <v>المشتقات</v>
       </c>
     </row>
-    <row r="155" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="155" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B155" s="1">
         <v>60</v>
       </c>
@@ -12312,7 +12320,7 @@
         <v>المشتقات</v>
       </c>
     </row>
-    <row r="156" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B156" s="1">
         <v>60</v>
       </c>
@@ -12355,7 +12363,7 @@
         <v>الأدب والنصوص جزء أول</v>
       </c>
     </row>
-    <row r="157" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="157" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B157" s="1">
         <v>60</v>
       </c>
@@ -12398,7 +12406,7 @@
         <v>الأدب والنصوص جزء أول</v>
       </c>
     </row>
-    <row r="158" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="158" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B158" s="1">
         <v>60</v>
       </c>
@@ -12441,7 +12449,7 @@
         <v>الأدب والنصوص جزء أول</v>
       </c>
     </row>
-    <row r="159" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="159" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B159" s="1">
         <v>60</v>
       </c>
@@ -12484,7 +12492,7 @@
         <v>الأدب والنصوص جزء أول</v>
       </c>
     </row>
-    <row r="160" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="160" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B160" s="1">
         <v>60</v>
       </c>
@@ -12527,7 +12535,7 @@
         <v>الأدب والنصوص جزء أول</v>
       </c>
     </row>
-    <row r="161" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="161" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B161" s="1">
         <v>60</v>
       </c>
@@ -12570,7 +12578,7 @@
         <v>الأدب والنصوص جزء أول</v>
       </c>
     </row>
-    <row r="162" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="162" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B162" s="1">
         <v>60</v>
       </c>
@@ -12613,7 +12621,7 @@
         <v>الأدب والنصوص جزء أول</v>
       </c>
     </row>
-    <row r="163" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="163" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B163" s="1">
         <v>60</v>
       </c>
@@ -12656,7 +12664,7 @@
         <v>الأدب والنصوص جزء أول</v>
       </c>
     </row>
-    <row r="164" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="164" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B164" s="1">
         <v>60</v>
       </c>
@@ -12699,7 +12707,7 @@
         <v>الأدب والنصوص جزء أول</v>
       </c>
     </row>
-    <row r="165" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="165" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B165" s="1">
         <v>60</v>
       </c>
@@ -12742,7 +12750,7 @@
         <v>الأدب والنصوص جزء أول</v>
       </c>
     </row>
-    <row r="166" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="166" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B166" s="1">
         <v>60</v>
       </c>
@@ -12785,7 +12793,7 @@
         <v>الأدب والنصوص جزء أول</v>
       </c>
     </row>
-    <row r="167" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="167" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B167" s="1">
         <v>60</v>
       </c>
@@ -12828,7 +12836,7 @@
         <v>الأدب والنصوص جزء أول</v>
       </c>
     </row>
-    <row r="168" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="168" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B168" s="1">
         <v>60</v>
       </c>
@@ -12871,7 +12879,7 @@
         <v>الأدب والنصوص جزء أول</v>
       </c>
     </row>
-    <row r="169" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="169" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B169" s="1">
         <v>60</v>
       </c>
@@ -12914,7 +12922,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="170" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="170" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B170" s="1">
         <v>60</v>
       </c>
@@ -12957,7 +12965,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="171" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="171" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B171" s="1">
         <v>60</v>
       </c>
@@ -13000,7 +13008,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="172" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="172" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B172" s="1">
         <v>60</v>
       </c>
@@ -13043,7 +13051,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="173" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="173" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B173" s="1">
         <v>60</v>
       </c>
@@ -13086,7 +13094,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="174" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="174" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B174" s="1">
         <v>60</v>
       </c>
@@ -13129,7 +13137,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="175" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="175" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B175" s="1">
         <v>60</v>
       </c>
@@ -13172,7 +13180,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="176" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="176" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B176" s="1">
         <v>60</v>
       </c>
@@ -13215,7 +13223,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="177" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="177" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B177" s="1">
         <v>60</v>
       </c>
@@ -13258,7 +13266,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="178" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="178" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B178" s="1">
         <v>60</v>
       </c>
@@ -13301,7 +13309,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="179" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="179" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B179" s="1">
         <v>60</v>
       </c>
@@ -13344,7 +13352,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="180" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="180" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B180" s="1">
         <v>60</v>
       </c>
@@ -13387,7 +13395,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="181" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="181" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B181" s="1">
         <v>60</v>
       </c>
@@ -13430,7 +13438,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="182" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="182" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B182" s="1">
         <v>60</v>
       </c>
@@ -13473,7 +13481,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="183" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="183" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B183" s="1">
         <v>60</v>
       </c>
@@ -13516,7 +13524,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="184" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="184" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B184" s="1">
         <v>60</v>
       </c>
@@ -13559,7 +13567,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="185" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="185" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B185" s="1">
         <v>60</v>
       </c>
@@ -13602,7 +13610,7 @@
         <v>الأدب والنصوص  جزء ثاني</v>
       </c>
     </row>
-    <row r="186" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="186" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B186" s="1">
         <v>60</v>
       </c>
@@ -13645,7 +13653,7 @@
         <v>البلاغة جزء أول</v>
       </c>
     </row>
-    <row r="187" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="187" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B187" s="1">
         <v>60</v>
       </c>
@@ -13688,7 +13696,7 @@
         <v>البلاغة جزء أول</v>
       </c>
     </row>
-    <row r="188" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="188" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B188" s="1">
         <v>60</v>
       </c>
@@ -13731,7 +13739,7 @@
         <v>البلاغة جزء أول</v>
       </c>
     </row>
-    <row r="189" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="189" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B189" s="1">
         <v>60</v>
       </c>
@@ -13774,7 +13782,7 @@
         <v>البلاغة جزء أول</v>
       </c>
     </row>
-    <row r="190" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="190" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B190" s="1">
         <v>60</v>
       </c>
@@ -13817,7 +13825,7 @@
         <v>البلاغة جزء أول</v>
       </c>
     </row>
-    <row r="191" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="191" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B191" s="1">
         <v>60</v>
       </c>
@@ -13860,7 +13868,7 @@
         <v>البلاغة جزء أول</v>
       </c>
     </row>
-    <row r="192" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="192" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B192" s="1">
         <v>60</v>
       </c>
@@ -13903,7 +13911,7 @@
         <v>البلاغة جزء أول</v>
       </c>
     </row>
-    <row r="193" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="193" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B193" s="1">
         <v>60</v>
       </c>
@@ -13946,7 +13954,7 @@
         <v>البلاغة جزء أول</v>
       </c>
     </row>
-    <row r="194" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="194" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B194" s="1">
         <v>60</v>
       </c>
@@ -13989,7 +13997,7 @@
         <v>البلاغة جزء أول</v>
       </c>
     </row>
-    <row r="195" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="195" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B195" s="1">
         <v>60</v>
       </c>
@@ -14032,7 +14040,7 @@
         <v>البلاغة جزء أول</v>
       </c>
     </row>
-    <row r="196" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="196" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B196" s="1">
         <v>60</v>
       </c>
@@ -14075,7 +14083,7 @@
         <v>البلاغة جزء ثاني</v>
       </c>
     </row>
-    <row r="197" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="197" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B197" s="1">
         <v>60</v>
       </c>
@@ -14118,7 +14126,7 @@
         <v>البلاغة جزء ثاني</v>
       </c>
     </row>
-    <row r="198" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="198" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B198" s="1">
         <v>60</v>
       </c>
@@ -14161,7 +14169,7 @@
         <v>البلاغة جزء ثاني</v>
       </c>
     </row>
-    <row r="199" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="199" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B199" s="1">
         <v>61</v>
       </c>
@@ -14204,7 +14212,7 @@
         <v>العروض</v>
       </c>
     </row>
-    <row r="200" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="200" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B200" s="1">
         <v>62</v>
       </c>
@@ -14247,7 +14255,7 @@
         <v>العروض</v>
       </c>
     </row>
-    <row r="201" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="201" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B201" s="1">
         <v>50</v>
       </c>
@@ -14290,7 +14298,7 @@
         <v>العروض ( 2 )</v>
       </c>
     </row>
-    <row r="202" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="202" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B202" s="1">
         <v>50</v>
       </c>
@@ -14333,7 +14341,7 @@
         <v>النحو  جزء أول</v>
       </c>
     </row>
-    <row r="203" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="203" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B203" s="1">
         <v>50</v>
       </c>
@@ -14376,7 +14384,7 @@
         <v>النحو  جزء أول</v>
       </c>
     </row>
-    <row r="204" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="204" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B204" s="1">
         <v>50</v>
       </c>
@@ -14419,7 +14427,7 @@
         <v>النحو  جزء أول</v>
       </c>
     </row>
-    <row r="205" spans="2:14" ht="92.5" x14ac:dyDescent="0.45">
+    <row r="205" spans="2:14" ht="90" x14ac:dyDescent="0.35">
       <c r="B205" s="1">
         <v>50</v>
       </c>
@@ -14462,7 +14470,7 @@
         <v>النحو  جزء أول</v>
       </c>
     </row>
-    <row r="206" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="206" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B206" s="1">
         <v>50</v>
       </c>
@@ -14505,7 +14513,7 @@
         <v>النحو  جزء أول</v>
       </c>
     </row>
-    <row r="207" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="207" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B207" s="1">
         <v>50</v>
       </c>
@@ -14548,7 +14556,7 @@
         <v>النحو  جزء أول</v>
       </c>
     </row>
-    <row r="208" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="208" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B208" s="1">
         <v>50</v>
       </c>
@@ -14591,7 +14599,7 @@
         <v>النحو  جزء أول</v>
       </c>
     </row>
-    <row r="209" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="209" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B209" s="1">
         <v>50</v>
       </c>
@@ -14634,7 +14642,7 @@
         <v>النحو  جزء أول</v>
       </c>
     </row>
-    <row r="210" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="210" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B210" s="1">
         <v>50</v>
       </c>
@@ -14677,7 +14685,7 @@
         <v>النحو  جزء أول</v>
       </c>
     </row>
-    <row r="211" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="211" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B211" s="1">
         <v>50</v>
       </c>
@@ -14720,7 +14728,7 @@
         <v>النحو  جزء أول</v>
       </c>
     </row>
-    <row r="212" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="212" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B212" s="1">
         <v>50</v>
       </c>
@@ -14763,7 +14771,7 @@
         <v>النحو  جزء أول</v>
       </c>
     </row>
-    <row r="213" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="213" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B213" s="1">
         <v>50</v>
       </c>
@@ -14806,7 +14814,7 @@
         <v>النحو  جزء أول</v>
       </c>
     </row>
-    <row r="214" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="214" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B214" s="1">
         <v>50</v>
       </c>
@@ -14849,7 +14857,7 @@
         <v>النحو  جزء أول</v>
       </c>
     </row>
-    <row r="215" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="215" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B215" s="1">
         <v>50</v>
       </c>
@@ -14892,7 +14900,7 @@
         <v>النحو  جزء أول</v>
       </c>
     </row>
-    <row r="216" spans="2:14" ht="92.5" x14ac:dyDescent="0.35">
+    <row r="216" spans="2:14" ht="90" x14ac:dyDescent="0.3">
       <c r="B216" s="1">
         <v>50</v>
       </c>
@@ -14935,7 +14943,7 @@
         <v>النحو جزء ثاني</v>
       </c>
     </row>
-    <row r="217" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="217" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B217" s="1">
         <v>50</v>
       </c>
@@ -14978,7 +14986,7 @@
         <v>النحو جزء ثاني</v>
       </c>
     </row>
-    <row r="218" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="218" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B218" s="1">
         <v>50</v>
       </c>
@@ -15021,7 +15029,7 @@
         <v>النحو جزء ثاني</v>
       </c>
     </row>
-    <row r="219" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="219" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B219" s="1">
         <v>50</v>
       </c>
@@ -15064,7 +15072,7 @@
         <v>النحو جزء ثاني</v>
       </c>
     </row>
-    <row r="220" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="220" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B220" s="1">
         <v>50</v>
       </c>
@@ -15107,7 +15115,7 @@
         <v>النحو جزء ثاني</v>
       </c>
     </row>
-    <row r="221" spans="2:14" ht="74" x14ac:dyDescent="0.35">
+    <row r="221" spans="2:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B221" s="1">
         <v>50</v>
       </c>
@@ -15150,7 +15158,7 @@
         <v>النحو جزء ثاني</v>
       </c>
     </row>
-    <row r="222" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="222" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B222" s="1">
         <v>50</v>
       </c>
@@ -15193,7 +15201,7 @@
         <v>النحو جزء ثاني</v>
       </c>
     </row>
-    <row r="223" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="223" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B223" s="1">
         <v>50</v>
       </c>
@@ -15236,7 +15244,7 @@
         <v>النحو جزء ثاني</v>
       </c>
     </row>
-    <row r="224" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="224" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B224" s="1">
         <v>50</v>
       </c>
@@ -15279,7 +15287,7 @@
         <v>النحو جزء ثاني</v>
       </c>
     </row>
-    <row r="225" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="225" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B225" s="1">
         <v>50</v>
       </c>
@@ -15322,7 +15330,7 @@
         <v>النحو جزء ثاني</v>
       </c>
     </row>
-    <row r="226" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="226" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B226" s="1">
         <v>50</v>
       </c>
@@ -15365,7 +15373,7 @@
         <v>النحو جزء ثاني</v>
       </c>
     </row>
-    <row r="227" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="227" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B227" s="1">
         <v>50</v>
       </c>
@@ -15408,7 +15416,7 @@
         <v>النحو جزء ثاني</v>
       </c>
     </row>
-    <row r="228" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="228" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B228" s="1">
         <v>50</v>
       </c>
@@ -15451,7 +15459,7 @@
         <v>النحو جزء ثاني</v>
       </c>
     </row>
-    <row r="229" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="229" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B229" s="1">
         <v>50</v>
       </c>
@@ -15494,7 +15502,7 @@
         <v xml:space="preserve">القراءة جزء أول </v>
       </c>
     </row>
-    <row r="230" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="230" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B230" s="1">
         <v>50</v>
       </c>
@@ -15537,7 +15545,7 @@
         <v xml:space="preserve">القراءة جزء أول </v>
       </c>
     </row>
-    <row r="231" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="231" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B231" s="1">
         <v>50</v>
       </c>
@@ -15580,7 +15588,7 @@
         <v xml:space="preserve">القراءة جزء أول </v>
       </c>
     </row>
-    <row r="232" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="232" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B232" s="1">
         <v>50</v>
       </c>
@@ -15623,7 +15631,7 @@
         <v xml:space="preserve">القراءة جزء أول </v>
       </c>
     </row>
-    <row r="233" spans="2:14" ht="92.5" x14ac:dyDescent="0.45">
+    <row r="233" spans="2:14" ht="90" x14ac:dyDescent="0.35">
       <c r="B233" s="1">
         <v>50</v>
       </c>
@@ -15666,7 +15674,7 @@
         <v xml:space="preserve">القراءة جزء أول </v>
       </c>
     </row>
-    <row r="234" spans="2:14" ht="92.5" x14ac:dyDescent="0.45">
+    <row r="234" spans="2:14" ht="90" x14ac:dyDescent="0.35">
       <c r="B234" s="1">
         <v>50</v>
       </c>
@@ -15709,7 +15717,7 @@
         <v xml:space="preserve">القراءة جزء أول </v>
       </c>
     </row>
-    <row r="235" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="235" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B235" s="1">
         <v>50</v>
       </c>
@@ -15752,7 +15760,7 @@
         <v xml:space="preserve">القراءة جزء أول </v>
       </c>
     </row>
-    <row r="236" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="236" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B236" s="1">
         <v>50</v>
       </c>
@@ -15795,7 +15803,7 @@
         <v xml:space="preserve">القراءة جزء أول </v>
       </c>
     </row>
-    <row r="237" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="237" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B237" s="1">
         <v>50</v>
       </c>
@@ -15838,7 +15846,7 @@
         <v>القراءة جزء ثاني</v>
       </c>
     </row>
-    <row r="238" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="238" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B238" s="1">
         <v>50</v>
       </c>
@@ -15881,7 +15889,7 @@
         <v>القراءة جزء ثاني</v>
       </c>
     </row>
-    <row r="239" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="239" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B239" s="1">
         <v>50</v>
       </c>
@@ -15924,7 +15932,7 @@
         <v>القراءة جزء ثاني</v>
       </c>
     </row>
-    <row r="240" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="240" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B240" s="1">
         <v>50</v>
       </c>
@@ -15967,7 +15975,7 @@
         <v>القراءة جزء ثاني</v>
       </c>
     </row>
-    <row r="241" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="241" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B241" s="1">
         <v>50</v>
       </c>
@@ -16010,7 +16018,7 @@
         <v>القراءة جزء ثاني</v>
       </c>
     </row>
-    <row r="242" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="242" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B242" s="1">
         <v>50</v>
       </c>
@@ -16053,7 +16061,7 @@
         <v>القراءة جزء ثاني</v>
       </c>
     </row>
-    <row r="243" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="243" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B243" s="1">
         <v>50</v>
       </c>
@@ -16096,7 +16104,7 @@
         <v>القراءة جزء ثاني</v>
       </c>
     </row>
-    <row r="244" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="244" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B244" s="1">
         <v>51</v>
       </c>
@@ -16139,7 +16147,7 @@
         <v>الإيمان  جزء أول</v>
       </c>
     </row>
-    <row r="245" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="245" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B245" s="1">
         <v>52</v>
       </c>
@@ -16182,7 +16190,7 @@
         <v>الإيمان  جزء أول</v>
       </c>
     </row>
-    <row r="246" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="246" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B246" s="1">
         <v>53</v>
       </c>
@@ -16225,7 +16233,7 @@
         <v>الإيمان  جزء أول</v>
       </c>
     </row>
-    <row r="247" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="247" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B247" s="1">
         <v>54</v>
       </c>
@@ -16268,7 +16276,7 @@
         <v>الإيمان  جزء أول</v>
       </c>
     </row>
-    <row r="248" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="248" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B248" s="1">
         <v>55</v>
       </c>
@@ -16311,7 +16319,7 @@
         <v>الإيمان  جزء أول</v>
       </c>
     </row>
-    <row r="249" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="249" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B249" s="1">
         <v>56</v>
       </c>
@@ -16354,7 +16362,7 @@
         <v>الإيمان  جزء أول</v>
       </c>
     </row>
-    <row r="250" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="250" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B250" s="1">
         <v>56</v>
       </c>
@@ -16397,7 +16405,7 @@
         <v>الإيمان جزء ثاني</v>
       </c>
     </row>
-    <row r="251" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="251" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B251" s="1">
         <v>56</v>
       </c>
@@ -16440,7 +16448,7 @@
         <v>الإيمان جزء ثاني</v>
       </c>
     </row>
-    <row r="252" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="252" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B252" s="1">
         <v>56</v>
       </c>
@@ -16483,7 +16491,7 @@
         <v>الإيمان جزء ثاني</v>
       </c>
     </row>
-    <row r="253" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="253" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B253" s="1">
         <v>56</v>
       </c>
@@ -16526,7 +16534,7 @@
         <v>الإيمان جزء ثاني</v>
       </c>
     </row>
-    <row r="254" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="254" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B254" s="1">
         <v>56</v>
       </c>
@@ -16569,7 +16577,7 @@
         <v>الإيمان جزء ثاني</v>
       </c>
     </row>
-    <row r="255" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="255" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B255" s="1">
         <v>56</v>
       </c>
@@ -16612,7 +16620,7 @@
         <v>الإيمان جزء ثاني</v>
       </c>
     </row>
-    <row r="256" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="256" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B256" s="1">
         <v>56</v>
       </c>
@@ -16655,7 +16663,7 @@
         <v>الإيمان جزء ثاني</v>
       </c>
     </row>
-    <row r="257" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="257" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B257" s="1">
         <v>50</v>
       </c>
@@ -16698,7 +16706,7 @@
         <v>الإيمان جزء ثاني</v>
       </c>
     </row>
-    <row r="258" spans="2:14" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="258" spans="2:14" ht="54" x14ac:dyDescent="0.3">
       <c r="B258" s="1">
         <v>50</v>
       </c>
@@ -16741,7 +16749,7 @@
         <v>الحديث  جزء أول</v>
       </c>
     </row>
-    <row r="259" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="259" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B259" s="1">
         <v>50</v>
       </c>
@@ -16784,7 +16792,7 @@
         <v>الحديث  جزء أول</v>
       </c>
     </row>
-    <row r="260" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="260" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B260" s="1">
         <v>50</v>
       </c>
@@ -16827,7 +16835,7 @@
         <v>الحديث  جزء أول</v>
       </c>
     </row>
-    <row r="261" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="261" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B261" s="1">
         <v>50</v>
       </c>
@@ -16870,7 +16878,7 @@
         <v>الحديث  جزء أول</v>
       </c>
     </row>
-    <row r="262" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="262" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B262" s="1">
         <v>50</v>
       </c>
@@ -16913,7 +16921,7 @@
         <v>الحديث  جزء أول</v>
       </c>
     </row>
-    <row r="263" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="263" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B263" s="1">
         <v>50</v>
       </c>
@@ -16956,7 +16964,7 @@
         <v>الحديث  جزء أول</v>
       </c>
     </row>
-    <row r="264" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="264" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B264" s="1">
         <v>50</v>
       </c>
@@ -16999,7 +17007,7 @@
         <v>الحديث  جزء أول</v>
       </c>
     </row>
-    <row r="265" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="265" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B265" s="1">
         <v>50</v>
       </c>
@@ -17042,7 +17050,7 @@
         <v>الحديث  جزء أول</v>
       </c>
     </row>
-    <row r="266" spans="2:14" ht="37" x14ac:dyDescent="0.35">
+    <row r="266" spans="2:14" ht="36" x14ac:dyDescent="0.3">
       <c r="B266" s="1">
         <v>50</v>
       </c>
@@ -17085,7 +17093,7 @@
         <v>الحديث جزء ثاني</v>
       </c>
     </row>
-    <row r="267" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="267" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B267" s="1">
         <v>50</v>
       </c>
@@ -17128,7 +17136,7 @@
         <v>الحديث جزء ثاني</v>
       </c>
     </row>
-    <row r="268" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="268" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B268" s="1">
         <v>50</v>
       </c>
@@ -17171,7 +17179,7 @@
         <v>الحديث جزء ثاني</v>
       </c>
     </row>
-    <row r="269" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="269" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B269" s="1">
         <v>50</v>
       </c>
@@ -17214,7 +17222,7 @@
         <v>الحديث جزء ثاني</v>
       </c>
     </row>
-    <row r="270" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="270" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B270" s="1">
         <v>50</v>
       </c>
@@ -17257,7 +17265,7 @@
         <v>الحديث جزء ثاني</v>
       </c>
     </row>
-    <row r="271" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="271" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B271" s="1">
         <v>50</v>
       </c>
@@ -17300,7 +17308,7 @@
         <v>الحديث جزء ثاني</v>
       </c>
     </row>
-    <row r="272" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="272" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B272" s="1">
         <v>50</v>
       </c>
@@ -17343,7 +17351,7 @@
         <v>الحديث جزء ثاني</v>
       </c>
     </row>
-    <row r="273" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="273" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B273" s="1">
         <v>50</v>
       </c>
@@ -17386,7 +17394,7 @@
         <v>الفقة جزء اول</v>
       </c>
     </row>
-    <row r="274" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="274" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B274" s="1">
         <v>50</v>
       </c>
@@ -17429,7 +17437,7 @@
         <v>الفقة جزء اول</v>
       </c>
     </row>
-    <row r="275" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="275" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B275" s="1">
         <v>50</v>
       </c>
@@ -17472,7 +17480,7 @@
         <v>الفقة جزء اول</v>
       </c>
     </row>
-    <row r="276" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="276" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B276" s="1">
         <v>50</v>
       </c>
@@ -17515,7 +17523,7 @@
         <v>الفقة جزء اول</v>
       </c>
     </row>
-    <row r="277" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="277" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B277" s="1">
         <v>50</v>
       </c>
@@ -17558,7 +17566,7 @@
         <v>الفقة جزء اول</v>
       </c>
     </row>
-    <row r="278" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="278" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B278" s="1">
         <v>50</v>
       </c>
@@ -17601,7 +17609,7 @@
         <v>الفقة جزء اول</v>
       </c>
     </row>
-    <row r="279" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="279" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B279" s="1">
         <v>50</v>
       </c>
@@ -17644,7 +17652,7 @@
         <v>الفقة جزء اول</v>
       </c>
     </row>
-    <row r="280" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="280" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B280" s="1">
         <v>50</v>
       </c>
@@ -17687,7 +17695,7 @@
         <v>الفقة جزء اول</v>
       </c>
     </row>
-    <row r="281" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="281" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B281" s="1">
         <v>50</v>
       </c>
@@ -17730,7 +17738,7 @@
         <v>الفقة جزء اول</v>
       </c>
     </row>
-    <row r="282" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="282" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B282" s="1">
         <v>50</v>
       </c>
@@ -17773,7 +17781,7 @@
         <v>الفقة جزء اول</v>
       </c>
     </row>
-    <row r="283" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="283" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B283" s="1">
         <v>50</v>
       </c>
@@ -17816,7 +17824,7 @@
         <v>الفقه جزء ثاني</v>
       </c>
     </row>
-    <row r="284" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="284" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B284" s="1">
         <v>50</v>
       </c>
@@ -17859,7 +17867,7 @@
         <v>الفقه جزء ثاني</v>
       </c>
     </row>
-    <row r="285" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="285" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B285" s="1">
         <v>50</v>
       </c>
@@ -17902,7 +17910,7 @@
         <v>الفقه جزء ثاني</v>
       </c>
     </row>
-    <row r="286" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="286" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B286" s="1">
         <v>50</v>
       </c>
@@ -17945,7 +17953,7 @@
         <v>الفقه جزء ثاني</v>
       </c>
     </row>
-    <row r="287" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="287" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B287" s="1">
         <v>50</v>
       </c>
@@ -17988,7 +17996,7 @@
         <v>الفقه جزء ثاني</v>
       </c>
     </row>
-    <row r="288" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="288" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B288" s="1">
         <v>50</v>
       </c>
@@ -18031,7 +18039,7 @@
         <v>الفقه جزء ثاني</v>
       </c>
     </row>
-    <row r="289" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="289" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B289" s="1">
         <v>50</v>
       </c>
@@ -18074,7 +18082,7 @@
         <v>الفقه جزء ثاني</v>
       </c>
     </row>
-    <row r="290" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="290" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B290" s="1">
         <v>50</v>
       </c>
@@ -18117,7 +18125,7 @@
         <v>الفقه جزء ثاني</v>
       </c>
     </row>
-    <row r="291" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="291" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B291" s="1">
         <v>50</v>
       </c>
@@ -18160,7 +18168,7 @@
         <v>الفقه جزء ثاني</v>
       </c>
     </row>
-    <row r="292" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="292" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B292" s="1">
         <v>50</v>
       </c>
@@ -18203,7 +18211,7 @@
         <v>الفقه جزء ثاني</v>
       </c>
     </row>
-    <row r="293" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="293" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B293" s="1">
         <v>50</v>
       </c>
@@ -18246,7 +18254,7 @@
         <v>الفقه جزء ثاني</v>
       </c>
     </row>
-    <row r="294" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="294" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B294" s="1">
         <v>50</v>
       </c>
@@ -18289,7 +18297,7 @@
         <v>السيرة جزء أول</v>
       </c>
     </row>
-    <row r="295" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="295" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B295" s="1">
         <v>50</v>
       </c>
@@ -18332,7 +18340,7 @@
         <v>السيرة جزء أول</v>
       </c>
     </row>
-    <row r="296" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="296" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B296" s="1">
         <v>50</v>
       </c>
@@ -18375,7 +18383,7 @@
         <v>السيرة جزء أول</v>
       </c>
     </row>
-    <row r="297" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="297" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B297" s="1">
         <v>50</v>
       </c>
@@ -18418,7 +18426,7 @@
         <v>السيرة جزء أول</v>
       </c>
     </row>
-    <row r="298" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="298" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B298" s="1">
         <v>50</v>
       </c>
@@ -18461,7 +18469,7 @@
         <v>السيرة جزء أول</v>
       </c>
     </row>
-    <row r="299" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="299" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B299" s="1">
         <v>50</v>
       </c>
@@ -18504,7 +18512,7 @@
         <v>السيرة جزء أول</v>
       </c>
     </row>
-    <row r="300" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="300" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B300" s="1">
         <v>50</v>
       </c>
@@ -18547,7 +18555,7 @@
         <v>السيرة جزء أول</v>
       </c>
     </row>
-    <row r="301" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="301" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B301" s="1">
         <v>50</v>
       </c>
@@ -18590,7 +18598,7 @@
         <v>السيرة جزء أول</v>
       </c>
     </row>
-    <row r="302" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="302" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B302" s="1">
         <v>50</v>
       </c>
@@ -18633,7 +18641,7 @@
         <v>السيرة النبوية جزء ثاني</v>
       </c>
     </row>
-    <row r="303" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="303" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B303" s="1">
         <v>50</v>
       </c>
@@ -18676,7 +18684,7 @@
         <v>السيرة النبوية جزء ثاني</v>
       </c>
     </row>
-    <row r="304" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="304" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B304" s="1">
         <v>50</v>
       </c>
@@ -18719,7 +18727,7 @@
         <v>السيرة النبوية جزء ثاني</v>
       </c>
     </row>
-    <row r="305" spans="2:14" ht="37" x14ac:dyDescent="0.45">
+    <row r="305" spans="2:14" ht="36" x14ac:dyDescent="0.35">
       <c r="B305" s="1">
         <v>50</v>
       </c>
@@ -18762,7 +18770,7 @@
         <v>السيرة النبوية جزء ثاني</v>
       </c>
     </row>
-    <row r="306" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="306" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B306" s="1">
         <v>50</v>
       </c>
@@ -18805,7 +18813,7 @@
         <v>السيرة النبوية جزء ثاني</v>
       </c>
     </row>
-    <row r="307" spans="2:14" ht="92.5" x14ac:dyDescent="0.45">
+    <row r="307" spans="2:14" ht="90" x14ac:dyDescent="0.35">
       <c r="B307" s="1">
         <v>50</v>
       </c>
@@ -18848,7 +18856,7 @@
         <v>السيرة النبوية جزء ثاني</v>
       </c>
     </row>
-    <row r="308" spans="2:14" ht="74" x14ac:dyDescent="0.45">
+    <row r="308" spans="2:14" ht="72" x14ac:dyDescent="0.35">
       <c r="B308" s="1">
         <v>50</v>
       </c>
@@ -18891,7 +18899,7 @@
         <v>السيرة النبوية جزء ثاني</v>
       </c>
     </row>
-    <row r="309" spans="2:14" ht="55.5" x14ac:dyDescent="0.45">
+    <row r="309" spans="2:14" ht="54" x14ac:dyDescent="0.35">
       <c r="B309" s="1">
         <v>50</v>
       </c>
@@ -18949,26 +18957,26 @@
       <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.90625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.08984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.08984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.6328125" style="12" customWidth="1"/>
-    <col min="13" max="13" width="61.26953125" style="12" customWidth="1"/>
-    <col min="14" max="14" width="5.7265625" style="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.08984375" style="11" customWidth="1"/>
-    <col min="16" max="16384" width="8.7265625" style="11"/>
+    <col min="1" max="1" width="45.88671875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.6640625" style="12" customWidth="1"/>
+    <col min="13" max="13" width="61.21875" style="12" customWidth="1"/>
+    <col min="14" max="14" width="5.77734375" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.109375" style="11" customWidth="1"/>
+    <col min="16" max="16384" width="8.77734375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -19015,7 +19023,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>35</v>
       </c>
@@ -19063,7 +19071,7 @@
         <v>مادة الجغرافيا ثاني أدبي</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="54" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>39</v>
       </c>
@@ -19111,7 +19119,7 @@
         <v>مادة الجغرافيا ثاني أدبي</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>42</v>
       </c>
@@ -19159,7 +19167,7 @@
         <v>مادة الجغرافيا ثاني أدبي</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>45</v>
       </c>
@@ -19207,7 +19215,7 @@
         <v>مادة الجغرافيا ثاني أدبي</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="54" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>48</v>
       </c>
@@ -19255,7 +19263,7 @@
         <v>مادة الجغرافيا ثاني أدبي</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="74" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>51</v>
       </c>
@@ -19303,7 +19311,7 @@
         <v>مادة الجغرافيا ثاني أدبي</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="37" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="54" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>54</v>
       </c>
@@ -19351,7 +19359,7 @@
         <v>مادة التاريخ ثاني أدبي</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="54" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>57</v>
       </c>
@@ -19399,7 +19407,7 @@
         <v>مادة التاريخ ثاني أدبي</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="74" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>60</v>
       </c>
@@ -19447,7 +19455,7 @@
         <v>مادة التاريخ ثاني أدبي</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="37" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>63</v>
       </c>
@@ -19495,7 +19503,7 @@
         <v>مادة علم الاجتماع ثاني أدبي</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="37" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>66</v>
       </c>
@@ -19543,7 +19551,7 @@
         <v>مادة علم الاجتماع ثاني أدبي</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="37" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>69</v>
       </c>
@@ -19591,7 +19599,7 @@
         <v>مادة علم الاجتماع ثاني أدبي</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="18" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>72</v>
       </c>
@@ -19639,7 +19647,7 @@
         <v>مادة علم الاجتماع ثاني أدبي</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>75</v>
       </c>
@@ -19687,7 +19695,7 @@
         <v>مادة علم الاجتماع ثاني أدبي</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="37" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>78</v>
       </c>
@@ -19735,7 +19743,7 @@
         <v>مادة علم الاجتماع ثاني أدبي</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="37" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" ht="36" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
         <v>81</v>
       </c>
@@ -19783,7 +19791,7 @@
         <v>مادة الاقتصاد ثاني أدبي</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="37" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" ht="36" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
         <v>84</v>
       </c>
@@ -19831,7 +19839,7 @@
         <v>مادة الاقتصاد ثاني أدبي</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
         <v>87</v>
       </c>
@@ -19879,7 +19887,7 @@
         <v>مادة الاقتصاد ثاني أدبي</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
         <v>90</v>
       </c>
@@ -19927,7 +19935,7 @@
         <v>مادة الاقتصاد ثاني أدبي</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="20" t="s">
         <v>93</v>
       </c>
@@ -19975,7 +19983,7 @@
         <v>مادة الاقتصاد ثاني أدبي</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="42" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A22" s="22" t="s">
         <v>96</v>
       </c>
@@ -20023,7 +20031,7 @@
         <v>مادة القرآن الكريم ثاني أدبي</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="42" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A23" s="22" t="s">
         <v>99</v>
       </c>
@@ -20071,7 +20079,7 @@
         <v>مادة القرآن الكريم ثاني أدبي</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A24" s="22" t="s">
         <v>102</v>
       </c>
@@ -20119,7 +20127,7 @@
         <v>مادة القرآن الكريم ثاني أدبي</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="42" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A25" s="22" t="s">
         <v>105</v>
       </c>
@@ -20167,7 +20175,7 @@
         <v>مادة القرآن الكريم ثاني أدبي</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A26" s="22" t="s">
         <v>108</v>
       </c>
@@ -20215,7 +20223,7 @@
         <v>مادة القرآن الكريم ثاني أدبي</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A27" s="22" t="s">
         <v>111</v>
       </c>
@@ -20263,7 +20271,7 @@
         <v>مادة القرآن الكريم ثاني أدبي</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>114</v>
       </c>
@@ -20311,7 +20319,7 @@
         <v>مادة مادة الرياضيات ثاني أدبي</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="37" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:15" ht="36" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>117</v>
       </c>
@@ -20359,7 +20367,7 @@
         <v>مادة مادة الرياضيات ثاني أدبي</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="37" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:15" ht="36" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
         <v>120</v>
       </c>
@@ -20407,7 +20415,7 @@
         <v>مادة مادة الرياضيات ثاني أدبي</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="37" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:15" ht="36" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>123</v>
       </c>
@@ -20455,7 +20463,7 @@
         <v>مادة مادة الرياضيات ثاني أدبي</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="37" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>126</v>
       </c>
@@ -20503,7 +20511,7 @@
         <v>مادة اللغة عربية ثاني أدبي</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="63" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" ht="63" x14ac:dyDescent="0.3">
       <c r="A33" s="25" t="s">
         <v>129</v>
       </c>
@@ -20551,7 +20559,7 @@
         <v>مادة اللغة عربية ثاني أدبي</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="37" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A34" s="25" t="s">
         <v>132</v>
       </c>
@@ -20599,7 +20607,7 @@
         <v>مادة اللغة عربية ثاني أدبي</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="37" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A35" s="25" t="s">
         <v>135</v>
       </c>
@@ -20647,7 +20655,7 @@
         <v>مادة اللغة عربية ثاني أدبي</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" ht="18" x14ac:dyDescent="0.3">
       <c r="A36" s="25" t="s">
         <v>138</v>
       </c>
@@ -20695,7 +20703,7 @@
         <v>مادة اللغة عربية ثاني أدبي</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" ht="18" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="s">
         <v>141</v>
       </c>
@@ -20743,7 +20751,7 @@
         <v>مادة اللغة عربية ثاني أدبي</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="74" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:15" ht="72" x14ac:dyDescent="0.35">
       <c r="A38" s="25" t="s">
         <v>144</v>
       </c>
@@ -20791,7 +20799,7 @@
         <v>مادة اللغة عربية ثاني أدبي</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="55.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" ht="54" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>147</v>
       </c>
@@ -20839,7 +20847,7 @@
         <v>مادة اللغة عربية ثاني أدبي</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="37" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" ht="36" x14ac:dyDescent="0.3">
       <c r="A40" s="25" t="s">
         <v>150</v>
       </c>
@@ -20887,7 +20895,7 @@
         <v>مادة اللغة عربية ثاني أدبي</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" ht="42" x14ac:dyDescent="0.3">
       <c r="A41" s="25" t="s">
         <v>153</v>
       </c>
@@ -20935,7 +20943,7 @@
         <v>مادة اللغة عربية ثاني أدبي</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="42" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:15" ht="42" x14ac:dyDescent="0.4">
       <c r="A42" s="31" t="s">
         <v>156</v>
       </c>
@@ -20983,7 +20991,7 @@
         <v>مادة الإسلامية ثاني أدبي</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="63" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" ht="63" x14ac:dyDescent="0.3">
       <c r="A43" s="31" t="s">
         <v>159</v>
       </c>
@@ -21031,7 +21039,7 @@
         <v>مادة الإسلامية ثاني أدبي</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="84" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" ht="84" x14ac:dyDescent="0.3">
       <c r="A44" s="31" t="s">
         <v>162</v>
       </c>
@@ -21079,7 +21087,7 @@
         <v>مادة الإسلامية ثاني أدبي</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="63" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:15" ht="63" x14ac:dyDescent="0.4">
       <c r="A45" s="31" t="s">
         <v>165</v>
       </c>
@@ -21127,7 +21135,7 @@
         <v>مادة الإسلامية ثاني أدبي</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:15" ht="63" x14ac:dyDescent="0.4">
       <c r="A46" s="31" t="s">
         <v>168</v>
       </c>
@@ -21175,7 +21183,7 @@
         <v>مادة الإسلامية ثاني أدبي</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="63" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:15" ht="63" x14ac:dyDescent="0.4">
       <c r="A47" s="31" t="s">
         <v>171</v>
       </c>
@@ -21223,7 +21231,7 @@
         <v>مادة الإسلامية ثاني أدبي</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="63" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:15" ht="84" x14ac:dyDescent="0.4">
       <c r="A48" s="31" t="s">
         <v>174</v>
       </c>
@@ -21271,7 +21279,7 @@
         <v>مادة الإسلامية ثاني أدبي</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="63" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:15" ht="63" x14ac:dyDescent="0.4">
       <c r="A49" s="31" t="s">
         <v>177</v>
       </c>
@@ -21329,28 +21337,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C2CBF8-9F0A-4ACB-8D4E-A066CEA18CA8}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.6328125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="44.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="15" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.6328125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="39.26953125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="25.54296875" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="3"/>
+    <col min="3" max="3" width="22.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="39.21875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="25.5546875" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="8.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -21388,12 +21396,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2">
-        <v>11</v>
+      <c r="B2" s="2" t="s">
+        <v>743</v>
       </c>
       <c r="C2" s="1">
         <v>120</v>
@@ -21426,12 +21434,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2">
-        <v>11</v>
+      <c r="B3" s="2" t="s">
+        <v>743</v>
       </c>
       <c r="C3" s="1">
         <v>120</v>
@@ -21464,12 +21472,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2">
-        <v>11</v>
+      <c r="B4" s="2" t="s">
+        <v>743</v>
       </c>
       <c r="C4" s="1">
         <v>120</v>
@@ -21502,12 +21510,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2">
-        <v>11</v>
+      <c r="B5" s="2" t="s">
+        <v>743</v>
       </c>
       <c r="C5" s="1">
         <v>120</v>
@@ -21540,12 +21548,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2">
-        <v>11</v>
+      <c r="B6" s="2" t="s">
+        <v>743</v>
       </c>
       <c r="C6" s="1">
         <v>120</v>
@@ -21578,12 +21586,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="2">
-        <v>11</v>
+      <c r="B7" s="2" t="s">
+        <v>743</v>
       </c>
       <c r="C7" s="1">
         <v>120</v>
@@ -21616,12 +21624,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2">
-        <v>11</v>
+      <c r="B8" s="2" t="s">
+        <v>743</v>
       </c>
       <c r="C8" s="1">
         <v>120</v>
@@ -21654,12 +21662,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="2">
-        <v>11</v>
+      <c r="B9" s="2" t="s">
+        <v>743</v>
       </c>
       <c r="C9" s="1">
         <v>120</v>

</xml_diff>